<commit_message>
handleError function on weight reducer.py
</commit_message>
<xml_diff>
--- a/imageDownloader/Image link extractor/jack snip projects/Lead tracker-20221025T204508Z-001/Lead tracker/vinmanager_20220613/data.xlsx
+++ b/imageDownloader/Image link extractor/jack snip projects/Lead tracker-20221025T204508Z-001/Lead tracker/vinmanager_20220613/data.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -421,42 +421,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Shap Sikandary</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>New_acfb - Remarketing Catalog - Ongoing</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>6/11 10:04 PM</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Your Internet Friends at Northland Volkswagen</t>
-        </is>
-      </c>
-    </row>
+    <row r="1"/>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Austin Allchurch</t>
+          <t>Asfiya Wasim
+2022 Volkswagen Taos (New)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Autoverify Lead - Trade</t>
+          <t>GUBAGOO - CHAT LEAD</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>6/13 8:54 PM</t>
+          <t>10/30 12:57 AM</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">

</xml_diff>

<commit_message>
Medium scraper tag updated
</commit_message>
<xml_diff>
--- a/imageDownloader/Image link extractor/jack snip projects/Lead tracker-20221025T204508Z-001/Lead tracker/vinmanager_20220613/data.xlsx
+++ b/imageDownloader/Image link extractor/jack snip projects/Lead tracker-20221025T204508Z-001/Lead tracker/vinmanager_20220613/data.xlsx
@@ -1,62 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rakib\PycharmProjects\UpworkPrljects-2\imageDownloader\Image link extractor\jack snip projects\Lead tracker-20221025T204508Z-001\Lead tracker\vinmanager_20220613\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2528D899-852F-4165-8D96-3E9DCBCDB82F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Asfiya Wasim
-2022 Volkswagen Taos (New)</t>
-  </si>
-  <si>
-    <t>GUBAGOO - CHAT LEAD</t>
-  </si>
-  <si>
-    <t>10/30 12:57 AM</t>
-  </si>
-  <si>
-    <t>Your Internet Friends at Northland Volkswagen</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -64,50 +42,85 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -395,119 +408,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Asfiya Wasim
+2022 Volkswagen Taos (New)</t>
+        </is>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>GUBAGOO - CHAT LEAD</t>
+        </is>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>10/30 12:57 AM</t>
+        </is>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Your Internet Friends at Northland Volkswagen</t>
+        </is>
       </c>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>